<commit_message>
add more function for to_excel()
</commit_message>
<xml_diff>
--- a/data/nonpay.xlsx
+++ b/data/nonpay.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="헬스비급여" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="헬스비급여_2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -694,6 +695,377 @@
           <t>PET진단료</t>
         </is>
       </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>캡슐내시경검사는 기존의 내시경검사로 접근이 곤란한 소장부위의 질환을 진단하기 위해 실시합니다. 평평하거나 침윤이 있거나, 염증이 있는 경우에는 기존의 방사선적 검사로 진단하는데 제한이 있어 이를 보완하기 위해 시행합니다.&lt;br&gt;&lt;br&gt;※ 아래 비용은 행위료와 재료대를 포함한 비용이므로 병원의 홈페이지 고지가격과 다를 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>캡슐내시경검사료</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>각종 진단서, 증명서 발급수수료를 말합니다. 일부 진단서는 진찰료가 별도로 발생할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>제증명수수료</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>E1100</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>환자의 질병명, 진단날짜, 치료내용, 의사성명 등이 기재&lt;br&gt;※  아래비용은 국문 제증명서 기준입니다.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>일반진단서</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>각종 진단서, 증명서 발급수수료를 말합니다. 일부 진단서는 진찰료가 별도로 발생할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>제증명수수료</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>E1200</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>개인의 사망을 증명하는 진단서로 사망원인, 사망일시, 사망장소 등이 기재. 의사가 환자를 진료한지 48시간 내에 예견된 원인으로 사망한 경우 발급 &lt;br&gt;※ 아래비용은 국문 제증명서 기준입니다.</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>사망진단서</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>1차분류코드</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>1차분류코드설명</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>1차분류코드명</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2차분류코드</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2차분류코드설명</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2차분류코드명</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>건강보험에서 정한 비용 외에 추가로 비용부담이 있는 병실입니다. (상급병실을 운영하는 병원은 일정규모의 보험적용 병실을 갖추어야 함) &lt;br&gt;※ 다만, 대형병원(상급종합병원)의 1인실 병실료는 건강보험 제외 대상입니다.  &lt;br&gt;▶ 특실, 출산 관련 병실, 정신과병실은 특수성을 감안하여 정보제공에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>상급병실료차액</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>A1100</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1개의 입원실에 1인 입원</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1인실</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>건강보험에서 정한 비용 외에 추가로 비용부담이 있는 병실입니다. (상급병실을 운영하는 병원은 일정규모의 보험적용 병실을 갖추어야 함) &lt;br&gt;※ 다만, 대형병원(상급종합병원)의 1인실 병실료는 건강보험 제외 대상입니다.  &lt;br&gt;▶ 특실, 출산 관련 병실, 정신과병실은 특수성을 감안하여 정보제공에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>상급병실료차액</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>A1200</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1개의 입원실에 2인 입원</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2인실</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>건강보험에서 정한 비용 외에 추가로 비용부담이 있는 병실입니다. (상급병실을 운영하는 병원은 일정규모의 보험적용 병실을 갖추어야 함) &lt;br&gt;※ 다만, 대형병원(상급종합병원)의 1인실 병실료는 건강보험 제외 대상입니다.  &lt;br&gt;▶ 특실, 출산 관련 병실, 정신과병실은 특수성을 감안하여 정보제공에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>상급병실료차액</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>A1300</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1개의 입원실에 3인 입원</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>3인실</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>초음파를 생성하는 탐촉자를 검사부위에 밀착시켜 초음파를 보낸 다음 되돌아오는 초음파를 실시간 영상화하는 검사입니다.&lt;br&gt;&lt;br&gt;※ 아래비용은 진단 목적으로 실시하는 검사로 추적검사는 공개비용에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>초음파검사료</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>B1100</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>물혹, 염증, 양성종양, 악성종양 등의 진단을 위해 실시하는 검사로 추적검사는 공개비용에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>갑상선(부갑상선포함)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>초음파를 생성하는 탐촉자를 검사부위에 밀착시켜 초음파를 보낸 다음 되돌아오는 초음파를 실시간 영상화하는 검사입니다.&lt;br&gt;&lt;br&gt;※ 아래비용은 진단 목적으로 실시하는 검사로 추적검사는 공개비용에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>초음파검사료</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>B1200</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>물혹, 염증, 양성고형종양, 악성종양 등의 진단을 위해 실시하는 검사로 추적검사는 공개비용에서 제외하였습니다</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>유방</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>초음파를 생성하는 탐촉자를 검사부위에 밀착시켜 초음파를 보낸 다음 되돌아오는 초음파를 실시간 영상화하는 검사입니다.&lt;br&gt;&lt;br&gt;※ 아래비용은 진단 목적으로 실시하는 검사로 추적검사는 공개비용에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>초음파검사료</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>B1300</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>물혹, 염증, 양성종양, 악성종양 등의 진단을 위해 실시하는 검사로 추적검사는 공개비용에서 제외하였습니다.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>상복부(간, 담낭, 담도, 비장, 췌장)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>양전자단층촬영(PET)은 양전자를 방출하는 방사성 동위원소(F-18 FDG)를 이용하여 인체의 생화학적, 물리학적 영상을 3차원으로 나타낼 수 있는 검사로, 전산화단층영상진단(CT)과 결합된 PET-CT로 검사하기도 합니다. &lt;br&gt;&lt;br&gt;※  아래 비용은 검사에 사용된 의약품과 재료 비용을 포함하므로 병원홈페이지의 고지가격과 상이할 수 있습니다. &lt;br&gt;     아울러, 동 검사료 이외에 영상저장 및 전송시스템료(Full PACS)가 추가로 발생할 수 있습니다.&lt;br&gt;   * "비고"의 조영제는 CT 조영제를 의미.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PET진단료</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>

</xml_diff>